<commit_message>
vault backup: 2026-01-03 18:50:58
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary.xlsx
+++ b/睡眠日记_Sleep_Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C3B183-62E1-4857-B1E2-4B9324EA5D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E8149B-8870-4E7E-9154-A5362E572ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="139">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -461,6 +461,43 @@
   </si>
   <si>
     <t>有 15：00-20：00</t>
+  </si>
+  <si>
+    <t>第一天
+日期:2025-1-03</t>
+  </si>
+  <si>
+    <t>第二天
+日期:2025-1-04</t>
+  </si>
+  <si>
+    <t>第三天
+日期:2025-1-05</t>
+  </si>
+  <si>
+    <t>第四天
+日期:2025-1-06</t>
+  </si>
+  <si>
+    <t>第五天
+日期:2025-1-07</t>
+  </si>
+  <si>
+    <t>第六天
+日期:2025-1-08</t>
+  </si>
+  <si>
+    <t>第七天
+日期:2025-1-09</t>
+  </si>
+  <si>
+    <t>6：47</t>
+  </si>
+  <si>
+    <t>6：55</t>
+  </si>
+  <si>
+    <t>12：30</t>
   </si>
 </sst>
 </file>
@@ -624,14 +661,6 @@
     <xf numFmtId="46" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -640,6 +669,14 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -943,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H117"/>
+  <dimension ref="A1:H135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="M115" sqref="M115"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B135" sqref="B135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
@@ -955,42 +992,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="10"/>
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
       <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:8" ht="16.5">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="14"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1384,42 +1421,42 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="10"/>
+      <c r="A21" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
       <c r="A22" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="10"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8" ht="16.5">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="14"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1810,42 +1847,42 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="10"/>
+      <c r="A40" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
       <c r="A41" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="10"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:8" ht="16.5">
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="14"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -2236,42 +2273,42 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="22.5">
-      <c r="A59" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B59" s="9"/>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="10"/>
+      <c r="A59" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="13"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
       <c r="A60" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="10"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="13"/>
     </row>
     <row r="61" spans="1:8" ht="16.5">
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="12" t="s">
+      <c r="B61" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
-      <c r="H61" s="14"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="10"/>
     </row>
     <row r="62" spans="1:8" ht="54">
       <c r="A62" s="2"/>
@@ -2665,27 +2702,27 @@
       <c r="A79" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B79" s="9"/>
-      <c r="C79" s="9"/>
-      <c r="D79" s="9"/>
-      <c r="E79" s="9"/>
-      <c r="F79" s="9"/>
-      <c r="G79" s="9"/>
-      <c r="H79" s="10"/>
+      <c r="B79" s="12"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="13"/>
     </row>
     <row r="80" spans="1:8" ht="16.5">
       <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B80" s="12" t="s">
+      <c r="B80" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="13"/>
-      <c r="D80" s="13"/>
-      <c r="E80" s="13"/>
-      <c r="F80" s="13"/>
-      <c r="G80" s="13"/>
-      <c r="H80" s="14"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="10"/>
     </row>
     <row r="81" spans="1:8" ht="54">
       <c r="A81" s="2"/>
@@ -3084,27 +3121,27 @@
       <c r="A101" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B101" s="9"/>
-      <c r="C101" s="9"/>
-      <c r="D101" s="9"/>
-      <c r="E101" s="9"/>
-      <c r="F101" s="9"/>
-      <c r="G101" s="9"/>
-      <c r="H101" s="10"/>
+      <c r="B101" s="12"/>
+      <c r="C101" s="12"/>
+      <c r="D101" s="12"/>
+      <c r="E101" s="12"/>
+      <c r="F101" s="12"/>
+      <c r="G101" s="12"/>
+      <c r="H101" s="13"/>
     </row>
     <row r="102" spans="1:8" ht="16.5">
       <c r="A102" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B102" s="12" t="s">
+      <c r="B102" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C102" s="13"/>
-      <c r="D102" s="13"/>
-      <c r="E102" s="13"/>
-      <c r="F102" s="13"/>
-      <c r="G102" s="13"/>
-      <c r="H102" s="14"/>
+      <c r="C102" s="9"/>
+      <c r="D102" s="9"/>
+      <c r="E102" s="9"/>
+      <c r="F102" s="9"/>
+      <c r="G102" s="9"/>
+      <c r="H102" s="10"/>
     </row>
     <row r="103" spans="1:8" ht="54">
       <c r="A103" s="2"/>
@@ -3494,24 +3531,272 @@
         <v>128</v>
       </c>
     </row>
+    <row r="119" spans="1:8" ht="17.25">
+      <c r="A119" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B119" s="12"/>
+      <c r="C119" s="12"/>
+      <c r="D119" s="12"/>
+      <c r="E119" s="12"/>
+      <c r="F119" s="12"/>
+      <c r="G119" s="12"/>
+      <c r="H119" s="13"/>
+    </row>
+    <row r="120" spans="1:8" ht="16.5">
+      <c r="A120" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C120" s="9"/>
+      <c r="D120" s="9"/>
+      <c r="E120" s="9"/>
+      <c r="F120" s="9"/>
+      <c r="G120" s="9"/>
+      <c r="H120" s="10"/>
+    </row>
+    <row r="121" spans="1:8" ht="36">
+      <c r="A121" s="2"/>
+      <c r="B121" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F121" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G121" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H121" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="33">
+      <c r="A122" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C122" s="6"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="6"/>
+      <c r="F122" s="6"/>
+      <c r="G122" s="6"/>
+      <c r="H122" s="6"/>
+    </row>
+    <row r="123" spans="1:8" ht="16.5">
+      <c r="A123" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C123" s="6"/>
+      <c r="D123" s="6"/>
+      <c r="E123" s="6"/>
+      <c r="F123" s="6"/>
+      <c r="G123" s="6"/>
+      <c r="H123" s="1"/>
+    </row>
+    <row r="124" spans="1:8" ht="16.5">
+      <c r="A124" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C124" s="6"/>
+      <c r="D124" s="6"/>
+      <c r="E124" s="7"/>
+      <c r="F124" s="6"/>
+      <c r="G124" s="6"/>
+      <c r="H124" s="1"/>
+    </row>
+    <row r="125" spans="1:8" ht="16.5">
+      <c r="A125" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C125" s="6"/>
+      <c r="D125" s="6"/>
+      <c r="E125" s="7"/>
+      <c r="F125" s="6"/>
+      <c r="G125" s="6"/>
+      <c r="H125" s="1"/>
+    </row>
+    <row r="126" spans="1:8" ht="49.5">
+      <c r="A126" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B126" s="6">
+        <v>0</v>
+      </c>
+      <c r="C126" s="1"/>
+      <c r="D126" s="7"/>
+      <c r="E126" s="1"/>
+      <c r="F126" s="1"/>
+      <c r="G126" s="1"/>
+      <c r="H126" s="1"/>
+    </row>
+    <row r="127" spans="1:8" ht="16.5">
+      <c r="A127" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B127" s="1">
+        <v>0</v>
+      </c>
+      <c r="C127" s="1"/>
+      <c r="D127" s="1"/>
+      <c r="E127" s="1"/>
+      <c r="F127" s="1"/>
+      <c r="G127" s="1"/>
+      <c r="H127" s="1"/>
+    </row>
+    <row r="128" spans="1:8" ht="33">
+      <c r="A128" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B128" s="1">
+        <v>0</v>
+      </c>
+      <c r="C128" s="1"/>
+      <c r="D128" s="1"/>
+      <c r="E128" s="1"/>
+      <c r="F128" s="1"/>
+      <c r="G128" s="1"/>
+      <c r="H128" s="1"/>
+    </row>
+    <row r="129" spans="1:8" ht="33">
+      <c r="A129" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B129" s="1">
+        <v>360</v>
+      </c>
+      <c r="C129" s="1"/>
+      <c r="D129" s="1"/>
+      <c r="E129" s="1"/>
+      <c r="F129" s="1"/>
+      <c r="G129" s="1"/>
+      <c r="H129" s="1"/>
+    </row>
+    <row r="130" spans="1:8" ht="82.5">
+      <c r="A130" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C130" s="1"/>
+      <c r="D130" s="1"/>
+      <c r="E130" s="1"/>
+      <c r="F130" s="1"/>
+      <c r="G130" s="1"/>
+      <c r="H130" s="1"/>
+    </row>
+    <row r="131" spans="1:8" ht="66">
+      <c r="A131" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B131" s="1">
+        <v>0</v>
+      </c>
+      <c r="C131" s="1"/>
+      <c r="D131" s="1"/>
+      <c r="E131" s="1"/>
+      <c r="F131" s="1"/>
+      <c r="G131" s="1"/>
+      <c r="H131" s="1"/>
+    </row>
+    <row r="132" spans="1:8" ht="49.5">
+      <c r="A132" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B132" s="1">
+        <v>4</v>
+      </c>
+      <c r="C132" s="1"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="1"/>
+      <c r="F132" s="1"/>
+      <c r="G132" s="1"/>
+      <c r="H132" s="1"/>
+    </row>
+    <row r="133" spans="1:8" ht="99">
+      <c r="A133" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B133" s="1">
+        <v>4</v>
+      </c>
+      <c r="C133" s="1"/>
+      <c r="D133" s="1"/>
+      <c r="E133" s="1"/>
+      <c r="F133" s="1"/>
+      <c r="G133" s="1"/>
+      <c r="H133" s="1"/>
+    </row>
+    <row r="134" spans="1:8" ht="115.5">
+      <c r="A134" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B134" s="1">
+        <v>4</v>
+      </c>
+      <c r="C134" s="1"/>
+      <c r="D134" s="1"/>
+      <c r="E134" s="1"/>
+      <c r="F134" s="1"/>
+      <c r="G134" s="1"/>
+      <c r="H134" s="1"/>
+    </row>
+    <row r="135" spans="1:8" ht="66">
+      <c r="A135" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C135" s="1"/>
+      <c r="D135" s="1"/>
+      <c r="E135" s="1"/>
+      <c r="F135" s="1"/>
+      <c r="G135" s="1"/>
+      <c r="H135" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="B102:H102"/>
-    <mergeCell ref="A79:H79"/>
-    <mergeCell ref="B80:H80"/>
-    <mergeCell ref="A101:H101"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="A21:H21"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A41:H41"/>
-    <mergeCell ref="B42:H42"/>
+  <mergeCells count="18">
+    <mergeCell ref="A119:H119"/>
+    <mergeCell ref="B120:H120"/>
     <mergeCell ref="A59:H59"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A60:H60"/>
     <mergeCell ref="A40:H40"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B102:H102"/>
+    <mergeCell ref="A79:H79"/>
+    <mergeCell ref="B80:H80"/>
+    <mergeCell ref="A101:H101"/>
+    <mergeCell ref="B61:H61"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
vault backup: 2026-01-05 10:47:37
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary.xlsx
+++ b/睡眠日记_Sleep_Diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E8149B-8870-4E7E-9154-A5362E572ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649FE5D4-0095-446D-8A9E-D24B9032B8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11040" yWindow="225" windowWidth="15705" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="睡眠日记 Sleep Diary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="143">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -497,7 +497,19 @@
     <t>6：55</t>
   </si>
   <si>
-    <t>12：30</t>
+    <t>7：57</t>
+  </si>
+  <si>
+    <t>5 min</t>
+  </si>
+  <si>
+    <t>10 ml 可乐 20：00</t>
+  </si>
+  <si>
+    <t>20 min</t>
+  </si>
+  <si>
+    <t>6 min</t>
   </si>
 </sst>
 </file>
@@ -661,6 +673,11 @@
     <xf numFmtId="46" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -670,11 +687,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -982,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B135" sqref="B135"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
@@ -995,39 +1007,39 @@
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8" ht="16.5">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="10"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1424,39 +1436,39 @@
       <c r="A21" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="13"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="13"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" ht="16.5">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="10"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1850,39 +1862,39 @@
       <c r="A40" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="13"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="13"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8" ht="16.5">
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="10"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="13"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -2276,39 +2288,39 @@
       <c r="A59" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B59" s="12"/>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
-      <c r="H59" s="13"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="10"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="11" t="s">
+      <c r="A60" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B60" s="12"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="13"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="10"/>
     </row>
     <row r="61" spans="1:8" ht="16.5">
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="8" t="s">
+      <c r="B61" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="10"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="13"/>
     </row>
     <row r="62" spans="1:8" ht="54">
       <c r="A62" s="2"/>
@@ -2699,30 +2711,30 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="17.25">
-      <c r="A79" s="11" t="s">
+      <c r="A79" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B79" s="12"/>
-      <c r="C79" s="12"/>
-      <c r="D79" s="12"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
-      <c r="G79" s="12"/>
-      <c r="H79" s="13"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="10"/>
     </row>
     <row r="80" spans="1:8" ht="16.5">
       <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="B80" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="9"/>
-      <c r="D80" s="9"/>
-      <c r="E80" s="9"/>
-      <c r="F80" s="9"/>
-      <c r="G80" s="9"/>
-      <c r="H80" s="10"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
+      <c r="H80" s="13"/>
     </row>
     <row r="81" spans="1:8" ht="54">
       <c r="A81" s="2"/>
@@ -3118,30 +3130,30 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="17.25">
-      <c r="A101" s="11" t="s">
+      <c r="A101" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B101" s="12"/>
-      <c r="C101" s="12"/>
-      <c r="D101" s="12"/>
-      <c r="E101" s="12"/>
-      <c r="F101" s="12"/>
-      <c r="G101" s="12"/>
-      <c r="H101" s="13"/>
+      <c r="B101" s="9"/>
+      <c r="C101" s="9"/>
+      <c r="D101" s="9"/>
+      <c r="E101" s="9"/>
+      <c r="F101" s="9"/>
+      <c r="G101" s="9"/>
+      <c r="H101" s="10"/>
     </row>
     <row r="102" spans="1:8" ht="16.5">
       <c r="A102" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B102" s="8" t="s">
+      <c r="B102" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C102" s="9"/>
-      <c r="D102" s="9"/>
-      <c r="E102" s="9"/>
-      <c r="F102" s="9"/>
-      <c r="G102" s="9"/>
-      <c r="H102" s="10"/>
+      <c r="C102" s="12"/>
+      <c r="D102" s="12"/>
+      <c r="E102" s="12"/>
+      <c r="F102" s="12"/>
+      <c r="G102" s="12"/>
+      <c r="H102" s="13"/>
     </row>
     <row r="103" spans="1:8" ht="54">
       <c r="A103" s="2"/>
@@ -3532,30 +3544,30 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="17.25">
-      <c r="A119" s="11" t="s">
+      <c r="A119" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B119" s="12"/>
-      <c r="C119" s="12"/>
-      <c r="D119" s="12"/>
-      <c r="E119" s="12"/>
-      <c r="F119" s="12"/>
-      <c r="G119" s="12"/>
-      <c r="H119" s="13"/>
+      <c r="B119" s="9"/>
+      <c r="C119" s="9"/>
+      <c r="D119" s="9"/>
+      <c r="E119" s="9"/>
+      <c r="F119" s="9"/>
+      <c r="G119" s="9"/>
+      <c r="H119" s="10"/>
     </row>
     <row r="120" spans="1:8" ht="16.5">
       <c r="A120" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B120" s="8" t="s">
+      <c r="B120" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C120" s="9"/>
-      <c r="D120" s="9"/>
-      <c r="E120" s="9"/>
-      <c r="F120" s="9"/>
-      <c r="G120" s="9"/>
-      <c r="H120" s="10"/>
+      <c r="C120" s="12"/>
+      <c r="D120" s="12"/>
+      <c r="E120" s="12"/>
+      <c r="F120" s="12"/>
+      <c r="G120" s="12"/>
+      <c r="H120" s="13"/>
     </row>
     <row r="121" spans="1:8" ht="36">
       <c r="A121" s="2"/>
@@ -3588,8 +3600,12 @@
       <c r="B122" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="C122" s="6"/>
-      <c r="D122" s="6"/>
+      <c r="C122" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D122" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="E122" s="6"/>
       <c r="F122" s="6"/>
       <c r="G122" s="6"/>
@@ -3602,8 +3618,12 @@
       <c r="B123" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="C123" s="6"/>
-      <c r="D123" s="6"/>
+      <c r="C123" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>16</v>
+      </c>
       <c r="E123" s="6"/>
       <c r="F123" s="6"/>
       <c r="G123" s="6"/>
@@ -3614,10 +3634,14 @@
         <v>5</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C124" s="6"/>
-      <c r="D124" s="6"/>
+        <v>63</v>
+      </c>
+      <c r="C124" s="6">
+        <v>0.9375</v>
+      </c>
+      <c r="D124" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="E124" s="7"/>
       <c r="F124" s="6"/>
       <c r="G124" s="6"/>
@@ -3628,10 +3652,14 @@
         <v>6</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C125" s="6"/>
-      <c r="D125" s="6"/>
+        <v>63</v>
+      </c>
+      <c r="C125" s="6">
+        <v>0.9375</v>
+      </c>
+      <c r="D125" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="E125" s="7"/>
       <c r="F125" s="6"/>
       <c r="G125" s="6"/>
@@ -3644,8 +3672,12 @@
       <c r="B126" s="6">
         <v>0</v>
       </c>
-      <c r="C126" s="1"/>
-      <c r="D126" s="7"/>
+      <c r="C126" s="1">
+        <v>5</v>
+      </c>
+      <c r="D126" s="7" t="s">
+        <v>139</v>
+      </c>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
@@ -3658,8 +3690,12 @@
       <c r="B127" s="1">
         <v>0</v>
       </c>
-      <c r="C127" s="1"/>
-      <c r="D127" s="1"/>
+      <c r="C127" s="1">
+        <v>0</v>
+      </c>
+      <c r="D127" s="1">
+        <v>2</v>
+      </c>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
@@ -3672,8 +3708,12 @@
       <c r="B128" s="1">
         <v>0</v>
       </c>
-      <c r="C128" s="1"/>
-      <c r="D128" s="1"/>
+      <c r="C128" s="1">
+        <v>0</v>
+      </c>
+      <c r="D128" s="1">
+        <v>20</v>
+      </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
@@ -3686,8 +3726,12 @@
       <c r="B129" s="1">
         <v>360</v>
       </c>
-      <c r="C129" s="1"/>
-      <c r="D129" s="1"/>
+      <c r="C129" s="1">
+        <v>570</v>
+      </c>
+      <c r="D129" s="1">
+        <v>480</v>
+      </c>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
@@ -3700,8 +3744,12 @@
       <c r="B130" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C130" s="1"/>
-      <c r="D130" s="1"/>
+      <c r="C130" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
@@ -3714,8 +3762,12 @@
       <c r="B131" s="1">
         <v>0</v>
       </c>
-      <c r="C131" s="1"/>
-      <c r="D131" s="1"/>
+      <c r="C131" s="1">
+        <v>0</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
@@ -3728,8 +3780,12 @@
       <c r="B132" s="1">
         <v>4</v>
       </c>
-      <c r="C132" s="1"/>
-      <c r="D132" s="1"/>
+      <c r="C132" s="1">
+        <v>4</v>
+      </c>
+      <c r="D132" s="1">
+        <v>4</v>
+      </c>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
@@ -3742,8 +3798,12 @@
       <c r="B133" s="1">
         <v>4</v>
       </c>
-      <c r="C133" s="1"/>
-      <c r="D133" s="1"/>
+      <c r="C133" s="1">
+        <v>4</v>
+      </c>
+      <c r="D133" s="1">
+        <v>4</v>
+      </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
@@ -3756,8 +3816,12 @@
       <c r="B134" s="1">
         <v>4</v>
       </c>
-      <c r="C134" s="1"/>
-      <c r="D134" s="1"/>
+      <c r="C134" s="1">
+        <v>4</v>
+      </c>
+      <c r="D134" s="1">
+        <v>4</v>
+      </c>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
@@ -3770,8 +3834,12 @@
       <c r="B135" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C135" s="1"/>
-      <c r="D135" s="1"/>
+      <c r="C135" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
@@ -3779,6 +3847,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A101:H101"/>
+    <mergeCell ref="B61:H61"/>
     <mergeCell ref="A119:H119"/>
     <mergeCell ref="B120:H120"/>
     <mergeCell ref="A59:H59"/>
@@ -3795,8 +3865,6 @@
     <mergeCell ref="B102:H102"/>
     <mergeCell ref="A79:H79"/>
     <mergeCell ref="B80:H80"/>
-    <mergeCell ref="A101:H101"/>
-    <mergeCell ref="B61:H61"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
vault backup: 2026-01-06 10:56:03
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary.xlsx
+++ b/睡眠日记_Sleep_Diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649FE5D4-0095-446D-8A9E-D24B9032B8E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C53954-4DB0-4211-A056-21380A9F4786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="225" windowWidth="15705" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11325" yWindow="195" windowWidth="15705" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="睡眠日记 Sleep Diary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="144">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -510,6 +510,9 @@
   </si>
   <si>
     <t>6 min</t>
+  </si>
+  <si>
+    <t>7：36</t>
   </si>
 </sst>
 </file>
@@ -994,8 +997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="C129" sqref="C129"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="F135" sqref="F135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
@@ -3606,7 +3609,9 @@
       <c r="D122" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E122" s="6"/>
+      <c r="E122" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="F122" s="6"/>
       <c r="G122" s="6"/>
       <c r="H122" s="6"/>
@@ -3624,7 +3629,9 @@
       <c r="D123" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E123" s="6"/>
+      <c r="E123" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="F123" s="6"/>
       <c r="G123" s="6"/>
       <c r="H123" s="1"/>
@@ -3642,7 +3649,9 @@
       <c r="D124" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E124" s="7"/>
+      <c r="E124" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="F124" s="6"/>
       <c r="G124" s="6"/>
       <c r="H124" s="1"/>
@@ -3660,7 +3669,9 @@
       <c r="D125" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E125" s="7"/>
+      <c r="E125" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="F125" s="6"/>
       <c r="G125" s="6"/>
       <c r="H125" s="1"/>
@@ -3678,7 +3689,9 @@
       <c r="D126" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E126" s="1"/>
+      <c r="E126" s="1">
+        <v>5</v>
+      </c>
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
@@ -3696,7 +3709,9 @@
       <c r="D127" s="1">
         <v>2</v>
       </c>
-      <c r="E127" s="1"/>
+      <c r="E127" s="1">
+        <v>2</v>
+      </c>
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
@@ -3714,7 +3729,9 @@
       <c r="D128" s="1">
         <v>20</v>
       </c>
-      <c r="E128" s="1"/>
+      <c r="E128" s="1">
+        <v>30</v>
+      </c>
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
@@ -3732,7 +3749,9 @@
       <c r="D129" s="1">
         <v>480</v>
       </c>
-      <c r="E129" s="1"/>
+      <c r="E129" s="1">
+        <v>490</v>
+      </c>
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
@@ -3750,7 +3769,9 @@
       <c r="D130" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E130" s="1"/>
+      <c r="E130" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
       <c r="H130" s="1"/>
@@ -3768,7 +3789,9 @@
       <c r="D131" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E131" s="1"/>
+      <c r="E131" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
@@ -3786,7 +3809,9 @@
       <c r="D132" s="1">
         <v>4</v>
       </c>
-      <c r="E132" s="1"/>
+      <c r="E132" s="1">
+        <v>4</v>
+      </c>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
@@ -3804,7 +3829,9 @@
       <c r="D133" s="1">
         <v>4</v>
       </c>
-      <c r="E133" s="1"/>
+      <c r="E133" s="1">
+        <v>3</v>
+      </c>
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
@@ -3822,7 +3849,9 @@
       <c r="D134" s="1">
         <v>4</v>
       </c>
-      <c r="E134" s="1"/>
+      <c r="E134" s="1">
+        <v>4</v>
+      </c>
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
@@ -3840,18 +3869,15 @@
       <c r="D135" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E135" s="1"/>
+      <c r="E135" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A101:H101"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="A119:H119"/>
-    <mergeCell ref="B120:H120"/>
-    <mergeCell ref="A59:H59"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A60:H60"/>
     <mergeCell ref="A40:H40"/>
@@ -3862,6 +3888,11 @@
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="A41:H41"/>
     <mergeCell ref="B42:H42"/>
+    <mergeCell ref="A101:H101"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="A119:H119"/>
+    <mergeCell ref="B120:H120"/>
+    <mergeCell ref="A59:H59"/>
     <mergeCell ref="B102:H102"/>
     <mergeCell ref="A79:H79"/>
     <mergeCell ref="B80:H80"/>

</xml_diff>

<commit_message>
vault backup: 2026-01-07 09:57:04
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary.xlsx
+++ b/睡眠日记_Sleep_Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C53954-4DB0-4211-A056-21380A9F4786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D93569A-6019-41E4-906B-13E44294E954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11325" yWindow="195" windowWidth="15705" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="144">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -676,11 +676,14 @@
     <xf numFmtId="46" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -689,9 +692,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -997,7 +997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <selection activeCell="F135" sqref="F135"/>
     </sheetView>
   </sheetViews>
@@ -1007,7 +1007,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
@@ -1019,7 +1019,7 @@
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9"/>
@@ -1034,15 +1034,15 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1436,7 +1436,7 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="9"/>
@@ -1448,7 +1448,7 @@
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="9"/>
@@ -1463,15 +1463,15 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1862,7 +1862,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="9"/>
@@ -1874,7 +1874,7 @@
       <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="9"/>
@@ -1889,15 +1889,15 @@
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="14"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -2288,7 +2288,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="22.5">
-      <c r="A59" s="14" t="s">
+      <c r="A59" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="9"/>
@@ -2300,7 +2300,7 @@
       <c r="H59" s="10"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="8" t="s">
+      <c r="A60" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="9"/>
@@ -2315,15 +2315,15 @@
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="B61" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="13"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="14"/>
     </row>
     <row r="62" spans="1:8" ht="54">
       <c r="A62" s="2"/>
@@ -2714,7 +2714,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="17.25">
-      <c r="A79" s="8" t="s">
+      <c r="A79" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B79" s="9"/>
@@ -2729,15 +2729,15 @@
       <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B80" s="11" t="s">
+      <c r="B80" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
-      <c r="G80" s="12"/>
-      <c r="H80" s="13"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="14"/>
     </row>
     <row r="81" spans="1:8" ht="54">
       <c r="A81" s="2"/>
@@ -3133,7 +3133,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="17.25">
-      <c r="A101" s="8" t="s">
+      <c r="A101" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B101" s="9"/>
@@ -3148,15 +3148,15 @@
       <c r="A102" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B102" s="11" t="s">
+      <c r="B102" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C102" s="12"/>
-      <c r="D102" s="12"/>
-      <c r="E102" s="12"/>
-      <c r="F102" s="12"/>
-      <c r="G102" s="12"/>
-      <c r="H102" s="13"/>
+      <c r="C102" s="13"/>
+      <c r="D102" s="13"/>
+      <c r="E102" s="13"/>
+      <c r="F102" s="13"/>
+      <c r="G102" s="13"/>
+      <c r="H102" s="14"/>
     </row>
     <row r="103" spans="1:8" ht="54">
       <c r="A103" s="2"/>
@@ -3547,7 +3547,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="17.25">
-      <c r="A119" s="8" t="s">
+      <c r="A119" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B119" s="9"/>
@@ -3562,15 +3562,15 @@
       <c r="A120" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B120" s="11" t="s">
+      <c r="B120" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C120" s="12"/>
-      <c r="D120" s="12"/>
-      <c r="E120" s="12"/>
-      <c r="F120" s="12"/>
-      <c r="G120" s="12"/>
-      <c r="H120" s="13"/>
+      <c r="C120" s="13"/>
+      <c r="D120" s="13"/>
+      <c r="E120" s="13"/>
+      <c r="F120" s="13"/>
+      <c r="G120" s="13"/>
+      <c r="H120" s="14"/>
     </row>
     <row r="121" spans="1:8" ht="36">
       <c r="A121" s="2"/>
@@ -3612,7 +3612,9 @@
       <c r="E122" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="F122" s="6"/>
+      <c r="F122" s="6">
+        <v>0.32430555555555557</v>
+      </c>
       <c r="G122" s="6"/>
       <c r="H122" s="6"/>
     </row>
@@ -3632,7 +3634,9 @@
       <c r="E123" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F123" s="6"/>
+      <c r="F123" s="6">
+        <v>0.34166666666666667</v>
+      </c>
       <c r="G123" s="6"/>
       <c r="H123" s="1"/>
     </row>
@@ -3652,7 +3656,9 @@
       <c r="E124" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F124" s="6"/>
+      <c r="F124" s="6">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="G124" s="6"/>
       <c r="H124" s="1"/>
     </row>
@@ -3672,7 +3678,9 @@
       <c r="E125" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F125" s="6"/>
+      <c r="F125" s="6">
+        <v>0.97916666666666663</v>
+      </c>
       <c r="G125" s="6"/>
       <c r="H125" s="1"/>
     </row>
@@ -3692,7 +3700,9 @@
       <c r="E126" s="1">
         <v>5</v>
       </c>
-      <c r="F126" s="1"/>
+      <c r="F126" s="1">
+        <v>5</v>
+      </c>
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
     </row>
@@ -3712,7 +3722,9 @@
       <c r="E127" s="1">
         <v>2</v>
       </c>
-      <c r="F127" s="1"/>
+      <c r="F127" s="1">
+        <v>1</v>
+      </c>
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
     </row>
@@ -3732,7 +3744,9 @@
       <c r="E128" s="1">
         <v>30</v>
       </c>
-      <c r="F128" s="1"/>
+      <c r="F128" s="1">
+        <v>6</v>
+      </c>
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
     </row>
@@ -3752,7 +3766,9 @@
       <c r="E129" s="1">
         <v>490</v>
       </c>
-      <c r="F129" s="1"/>
+      <c r="F129" s="1">
+        <v>480</v>
+      </c>
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
     </row>
@@ -3772,7 +3788,9 @@
       <c r="E130" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F130" s="1"/>
+      <c r="F130" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="G130" s="1"/>
       <c r="H130" s="1"/>
     </row>
@@ -3792,7 +3810,9 @@
       <c r="E131" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F131" s="1"/>
+      <c r="F131" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
     </row>
@@ -3812,7 +3832,9 @@
       <c r="E132" s="1">
         <v>4</v>
       </c>
-      <c r="F132" s="1"/>
+      <c r="F132" s="1">
+        <v>3</v>
+      </c>
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
     </row>
@@ -3832,7 +3854,9 @@
       <c r="E133" s="1">
         <v>3</v>
       </c>
-      <c r="F133" s="1"/>
+      <c r="F133" s="1">
+        <v>4</v>
+      </c>
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
     </row>
@@ -3852,7 +3876,9 @@
       <c r="E134" s="1">
         <v>4</v>
       </c>
-      <c r="F134" s="1"/>
+      <c r="F134" s="1">
+        <v>3</v>
+      </c>
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
     </row>
@@ -3872,12 +3898,22 @@
       <c r="E135" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F135" s="1"/>
+      <c r="F135" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A101:H101"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="A119:H119"/>
+    <mergeCell ref="B120:H120"/>
+    <mergeCell ref="A59:H59"/>
+    <mergeCell ref="B102:H102"/>
+    <mergeCell ref="A79:H79"/>
+    <mergeCell ref="B80:H80"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A60:H60"/>
     <mergeCell ref="A40:H40"/>
@@ -3888,14 +3924,6 @@
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="A41:H41"/>
     <mergeCell ref="B42:H42"/>
-    <mergeCell ref="A101:H101"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="A119:H119"/>
-    <mergeCell ref="B120:H120"/>
-    <mergeCell ref="A59:H59"/>
-    <mergeCell ref="B102:H102"/>
-    <mergeCell ref="A79:H79"/>
-    <mergeCell ref="B80:H80"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
vault backup: 2026-01-08 11:23:03
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary.xlsx
+++ b/睡眠日记_Sleep_Diary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D93569A-6019-41E4-906B-13E44294E954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A2A9DA-3D00-48A2-8D28-1DB7E500385A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11325" yWindow="195" windowWidth="15705" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="睡眠日记 Sleep Diary" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="145">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -513,6 +513,9 @@
   </si>
   <si>
     <t>7：36</t>
+  </si>
+  <si>
+    <t>7：22</t>
   </si>
 </sst>
 </file>
@@ -676,14 +679,11 @@
     <xf numFmtId="46" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -692,6 +692,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -997,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="F135" sqref="F135"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="G135" sqref="G135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
@@ -1007,7 +1010,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
@@ -1019,7 +1022,7 @@
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="9"/>
@@ -1034,15 +1037,15 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="14"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1436,7 +1439,7 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="9"/>
@@ -1448,7 +1451,7 @@
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="9"/>
@@ -1463,15 +1466,15 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="14"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1862,7 +1865,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="9"/>
@@ -1874,7 +1877,7 @@
       <c r="H40" s="10"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="9"/>
@@ -1889,15 +1892,15 @@
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="14"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="13"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -2288,7 +2291,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="22.5">
-      <c r="A59" s="8" t="s">
+      <c r="A59" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="9"/>
@@ -2300,7 +2303,7 @@
       <c r="H59" s="10"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="11" t="s">
+      <c r="A60" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="9"/>
@@ -2315,15 +2318,15 @@
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="12" t="s">
+      <c r="B61" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
-      <c r="H61" s="14"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="13"/>
     </row>
     <row r="62" spans="1:8" ht="54">
       <c r="A62" s="2"/>
@@ -2714,7 +2717,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="17.25">
-      <c r="A79" s="11" t="s">
+      <c r="A79" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B79" s="9"/>
@@ -2729,15 +2732,15 @@
       <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B80" s="12" t="s">
+      <c r="B80" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="13"/>
-      <c r="D80" s="13"/>
-      <c r="E80" s="13"/>
-      <c r="F80" s="13"/>
-      <c r="G80" s="13"/>
-      <c r="H80" s="14"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
+      <c r="H80" s="13"/>
     </row>
     <row r="81" spans="1:8" ht="54">
       <c r="A81" s="2"/>
@@ -3133,7 +3136,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="17.25">
-      <c r="A101" s="11" t="s">
+      <c r="A101" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B101" s="9"/>
@@ -3148,15 +3151,15 @@
       <c r="A102" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B102" s="12" t="s">
+      <c r="B102" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C102" s="13"/>
-      <c r="D102" s="13"/>
-      <c r="E102" s="13"/>
-      <c r="F102" s="13"/>
-      <c r="G102" s="13"/>
-      <c r="H102" s="14"/>
+      <c r="C102" s="12"/>
+      <c r="D102" s="12"/>
+      <c r="E102" s="12"/>
+      <c r="F102" s="12"/>
+      <c r="G102" s="12"/>
+      <c r="H102" s="13"/>
     </row>
     <row r="103" spans="1:8" ht="54">
       <c r="A103" s="2"/>
@@ -3547,7 +3550,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="17.25">
-      <c r="A119" s="11" t="s">
+      <c r="A119" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B119" s="9"/>
@@ -3562,15 +3565,15 @@
       <c r="A120" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B120" s="12" t="s">
+      <c r="B120" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C120" s="13"/>
-      <c r="D120" s="13"/>
-      <c r="E120" s="13"/>
-      <c r="F120" s="13"/>
-      <c r="G120" s="13"/>
-      <c r="H120" s="14"/>
+      <c r="C120" s="12"/>
+      <c r="D120" s="12"/>
+      <c r="E120" s="12"/>
+      <c r="F120" s="12"/>
+      <c r="G120" s="12"/>
+      <c r="H120" s="13"/>
     </row>
     <row r="121" spans="1:8" ht="36">
       <c r="A121" s="2"/>
@@ -3615,7 +3618,9 @@
       <c r="F122" s="6">
         <v>0.32430555555555557</v>
       </c>
-      <c r="G122" s="6"/>
+      <c r="G122" s="6" t="s">
+        <v>144</v>
+      </c>
       <c r="H122" s="6"/>
     </row>
     <row r="123" spans="1:8" ht="16.5">
@@ -3637,7 +3642,9 @@
       <c r="F123" s="6">
         <v>0.34166666666666667</v>
       </c>
-      <c r="G123" s="6"/>
+      <c r="G123" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="H123" s="1"/>
     </row>
     <row r="124" spans="1:8" ht="16.5">
@@ -3659,7 +3666,9 @@
       <c r="F124" s="6">
         <v>0.97916666666666663</v>
       </c>
-      <c r="G124" s="6"/>
+      <c r="G124" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="H124" s="1"/>
     </row>
     <row r="125" spans="1:8" ht="16.5">
@@ -3681,7 +3690,9 @@
       <c r="F125" s="6">
         <v>0.97916666666666663</v>
       </c>
-      <c r="G125" s="6"/>
+      <c r="G125" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="H125" s="1"/>
     </row>
     <row r="126" spans="1:8" ht="49.5">
@@ -3703,7 +3714,9 @@
       <c r="F126" s="1">
         <v>5</v>
       </c>
-      <c r="G126" s="1"/>
+      <c r="G126" s="1">
+        <v>5</v>
+      </c>
       <c r="H126" s="1"/>
     </row>
     <row r="127" spans="1:8" ht="16.5">
@@ -3725,7 +3738,9 @@
       <c r="F127" s="1">
         <v>1</v>
       </c>
-      <c r="G127" s="1"/>
+      <c r="G127" s="1">
+        <v>0</v>
+      </c>
       <c r="H127" s="1"/>
     </row>
     <row r="128" spans="1:8" ht="33">
@@ -3747,7 +3762,9 @@
       <c r="F128" s="1">
         <v>6</v>
       </c>
-      <c r="G128" s="1"/>
+      <c r="G128" s="1">
+        <v>0</v>
+      </c>
       <c r="H128" s="1"/>
     </row>
     <row r="129" spans="1:8" ht="33">
@@ -3769,7 +3786,9 @@
       <c r="F129" s="1">
         <v>480</v>
       </c>
-      <c r="G129" s="1"/>
+      <c r="G129" s="1">
+        <v>480</v>
+      </c>
       <c r="H129" s="1"/>
     </row>
     <row r="130" spans="1:8" ht="82.5">
@@ -3791,7 +3810,9 @@
       <c r="F130" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G130" s="1"/>
+      <c r="G130" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="H130" s="1"/>
     </row>
     <row r="131" spans="1:8" ht="66">
@@ -3813,7 +3834,9 @@
       <c r="F131" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G131" s="1"/>
+      <c r="G131" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="H131" s="1"/>
     </row>
     <row r="132" spans="1:8" ht="49.5">
@@ -3835,7 +3858,9 @@
       <c r="F132" s="1">
         <v>3</v>
       </c>
-      <c r="G132" s="1"/>
+      <c r="G132" s="1">
+        <v>4</v>
+      </c>
       <c r="H132" s="1"/>
     </row>
     <row r="133" spans="1:8" ht="99">
@@ -3857,7 +3882,9 @@
       <c r="F133" s="1">
         <v>4</v>
       </c>
-      <c r="G133" s="1"/>
+      <c r="G133" s="1">
+        <v>4</v>
+      </c>
       <c r="H133" s="1"/>
     </row>
     <row r="134" spans="1:8" ht="115.5">
@@ -3879,7 +3906,9 @@
       <c r="F134" s="1">
         <v>3</v>
       </c>
-      <c r="G134" s="1"/>
+      <c r="G134" s="1">
+        <v>4</v>
+      </c>
       <c r="H134" s="1"/>
     </row>
     <row r="135" spans="1:8" ht="66">
@@ -3901,19 +3930,13 @@
       <c r="F135" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G135" s="1"/>
+      <c r="G135" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="H135" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A101:H101"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="A119:H119"/>
-    <mergeCell ref="B120:H120"/>
-    <mergeCell ref="A59:H59"/>
-    <mergeCell ref="B102:H102"/>
-    <mergeCell ref="A79:H79"/>
-    <mergeCell ref="B80:H80"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A60:H60"/>
     <mergeCell ref="A40:H40"/>
@@ -3924,6 +3947,14 @@
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="A41:H41"/>
     <mergeCell ref="B42:H42"/>
+    <mergeCell ref="A101:H101"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="A119:H119"/>
+    <mergeCell ref="B120:H120"/>
+    <mergeCell ref="A59:H59"/>
+    <mergeCell ref="B102:H102"/>
+    <mergeCell ref="A79:H79"/>
+    <mergeCell ref="B80:H80"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
vault backup: 2026-01-09 10:05:50
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary.xlsx
+++ b/睡眠日记_Sleep_Diary.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A2A9DA-3D00-48A2-8D28-1DB7E500385A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8E0001-9F8B-48C5-B61A-77F6A6E80FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11865" yWindow="225" windowWidth="15705" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="睡眠日记 Sleep Diary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="154">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -516,6 +527,33 @@
   </si>
   <si>
     <t>7：22</t>
+  </si>
+  <si>
+    <t>6：38</t>
+  </si>
+  <si>
+    <t>22：52</t>
+  </si>
+  <si>
+    <t>第一天</t>
+  </si>
+  <si>
+    <t>第二天</t>
+  </si>
+  <si>
+    <t>第三天</t>
+  </si>
+  <si>
+    <t>第四天</t>
+  </si>
+  <si>
+    <t>第五天</t>
+  </si>
+  <si>
+    <t>第六天</t>
+  </si>
+  <si>
+    <t>第七天</t>
   </si>
 </sst>
 </file>
@@ -656,7 +694,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -679,11 +717,6 @@
     <xf numFmtId="46" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -695,6 +728,23 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -998,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H135"/>
+  <dimension ref="A1:H155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="G135" sqref="G135"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="E145" sqref="E145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
@@ -1010,42 +1060,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="10"/>
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="13"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:8" ht="16.5">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="17"/>
     </row>
     <row r="4" spans="1:8" ht="54">
       <c r="A4" s="2"/>
@@ -1439,42 +1489,42 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="10"/>
+      <c r="A21" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="10"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8" ht="16.5">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="13"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="17"/>
     </row>
     <row r="24" spans="1:8" ht="54">
       <c r="A24" s="2"/>
@@ -1865,42 +1915,42 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="10"/>
+      <c r="A40" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="10"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:8" ht="16.5">
       <c r="A42" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="13"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="17"/>
     </row>
     <row r="43" spans="1:8" ht="54">
       <c r="A43" s="2"/>
@@ -2291,42 +2341,42 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="22.5">
-      <c r="A59" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B59" s="9"/>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="10"/>
+      <c r="A59" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="13"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="8" t="s">
+      <c r="A60" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="10"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="13"/>
     </row>
     <row r="61" spans="1:8" ht="16.5">
       <c r="A61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="B61" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="13"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="16"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="17"/>
     </row>
     <row r="62" spans="1:8" ht="54">
       <c r="A62" s="2"/>
@@ -2717,30 +2767,30 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="17.25">
-      <c r="A79" s="8" t="s">
+      <c r="A79" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B79" s="9"/>
-      <c r="C79" s="9"/>
-      <c r="D79" s="9"/>
-      <c r="E79" s="9"/>
-      <c r="F79" s="9"/>
-      <c r="G79" s="9"/>
-      <c r="H79" s="10"/>
+      <c r="B79" s="12"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="13"/>
     </row>
     <row r="80" spans="1:8" ht="16.5">
       <c r="A80" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B80" s="11" t="s">
+      <c r="B80" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
-      <c r="G80" s="12"/>
-      <c r="H80" s="13"/>
+      <c r="C80" s="16"/>
+      <c r="D80" s="16"/>
+      <c r="E80" s="16"/>
+      <c r="F80" s="16"/>
+      <c r="G80" s="16"/>
+      <c r="H80" s="17"/>
     </row>
     <row r="81" spans="1:8" ht="54">
       <c r="A81" s="2"/>
@@ -3136,30 +3186,30 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="17.25">
-      <c r="A101" s="8" t="s">
+      <c r="A101" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B101" s="9"/>
-      <c r="C101" s="9"/>
-      <c r="D101" s="9"/>
-      <c r="E101" s="9"/>
-      <c r="F101" s="9"/>
-      <c r="G101" s="9"/>
-      <c r="H101" s="10"/>
+      <c r="B101" s="12"/>
+      <c r="C101" s="12"/>
+      <c r="D101" s="12"/>
+      <c r="E101" s="12"/>
+      <c r="F101" s="12"/>
+      <c r="G101" s="12"/>
+      <c r="H101" s="13"/>
     </row>
     <row r="102" spans="1:8" ht="16.5">
       <c r="A102" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B102" s="11" t="s">
+      <c r="B102" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C102" s="12"/>
-      <c r="D102" s="12"/>
-      <c r="E102" s="12"/>
-      <c r="F102" s="12"/>
-      <c r="G102" s="12"/>
-      <c r="H102" s="13"/>
+      <c r="C102" s="16"/>
+      <c r="D102" s="16"/>
+      <c r="E102" s="16"/>
+      <c r="F102" s="16"/>
+      <c r="G102" s="16"/>
+      <c r="H102" s="17"/>
     </row>
     <row r="103" spans="1:8" ht="54">
       <c r="A103" s="2"/>
@@ -3550,30 +3600,30 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="17.25">
-      <c r="A119" s="8" t="s">
+      <c r="A119" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B119" s="9"/>
-      <c r="C119" s="9"/>
-      <c r="D119" s="9"/>
-      <c r="E119" s="9"/>
-      <c r="F119" s="9"/>
-      <c r="G119" s="9"/>
-      <c r="H119" s="10"/>
+      <c r="B119" s="12"/>
+      <c r="C119" s="12"/>
+      <c r="D119" s="12"/>
+      <c r="E119" s="12"/>
+      <c r="F119" s="12"/>
+      <c r="G119" s="12"/>
+      <c r="H119" s="13"/>
     </row>
     <row r="120" spans="1:8" ht="16.5">
       <c r="A120" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B120" s="11" t="s">
+      <c r="B120" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C120" s="12"/>
-      <c r="D120" s="12"/>
-      <c r="E120" s="12"/>
-      <c r="F120" s="12"/>
-      <c r="G120" s="12"/>
-      <c r="H120" s="13"/>
+      <c r="C120" s="16"/>
+      <c r="D120" s="16"/>
+      <c r="E120" s="16"/>
+      <c r="F120" s="16"/>
+      <c r="G120" s="16"/>
+      <c r="H120" s="17"/>
     </row>
     <row r="121" spans="1:8" ht="36">
       <c r="A121" s="2"/>
@@ -3621,7 +3671,9 @@
       <c r="G122" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="H122" s="6"/>
+      <c r="H122" s="6" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="123" spans="1:8" ht="16.5">
       <c r="A123" s="1" t="s">
@@ -3645,7 +3697,9 @@
       <c r="G123" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H123" s="1"/>
+      <c r="H123" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="124" spans="1:8" ht="16.5">
       <c r="A124" s="1" t="s">
@@ -3669,7 +3723,9 @@
       <c r="G124" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H124" s="1"/>
+      <c r="H124" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="125" spans="1:8" ht="16.5">
       <c r="A125" s="1" t="s">
@@ -3693,7 +3749,9 @@
       <c r="G125" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="H125" s="1"/>
+      <c r="H125" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="126" spans="1:8" ht="49.5">
       <c r="A126" s="1" t="s">
@@ -3717,7 +3775,9 @@
       <c r="G126" s="1">
         <v>5</v>
       </c>
-      <c r="H126" s="1"/>
+      <c r="H126" s="1">
+        <v>15</v>
+      </c>
     </row>
     <row r="127" spans="1:8" ht="16.5">
       <c r="A127" s="1" t="s">
@@ -3741,7 +3801,9 @@
       <c r="G127" s="1">
         <v>0</v>
       </c>
-      <c r="H127" s="1"/>
+      <c r="H127" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="128" spans="1:8" ht="33">
       <c r="A128" s="1" t="s">
@@ -3765,7 +3827,9 @@
       <c r="G128" s="1">
         <v>0</v>
       </c>
-      <c r="H128" s="1"/>
+      <c r="H128" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="129" spans="1:8" ht="33">
       <c r="A129" s="1" t="s">
@@ -3789,7 +3853,9 @@
       <c r="G129" s="1">
         <v>480</v>
       </c>
-      <c r="H129" s="1"/>
+      <c r="H129" s="1">
+        <v>470</v>
+      </c>
     </row>
     <row r="130" spans="1:8" ht="82.5">
       <c r="A130" s="1" t="s">
@@ -3813,7 +3879,9 @@
       <c r="G130" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H130" s="1"/>
+      <c r="H130" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="131" spans="1:8" ht="66">
       <c r="A131" s="1" t="s">
@@ -3837,7 +3905,9 @@
       <c r="G131" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H131" s="1"/>
+      <c r="H131" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="132" spans="1:8" ht="49.5">
       <c r="A132" s="1" t="s">
@@ -3861,7 +3931,9 @@
       <c r="G132" s="1">
         <v>4</v>
       </c>
-      <c r="H132" s="1"/>
+      <c r="H132" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="133" spans="1:8" ht="99">
       <c r="A133" s="1" t="s">
@@ -3885,7 +3957,9 @@
       <c r="G133" s="1">
         <v>4</v>
       </c>
-      <c r="H133" s="1"/>
+      <c r="H133" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="134" spans="1:8" ht="115.5">
       <c r="A134" s="1" t="s">
@@ -3909,7 +3983,9 @@
       <c r="G134" s="1">
         <v>4</v>
       </c>
-      <c r="H134" s="1"/>
+      <c r="H134" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="135" spans="1:8" ht="66">
       <c r="A135" s="1" t="s">
@@ -3933,10 +4009,270 @@
       <c r="G135" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H135" s="1"/>
+      <c r="H135" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" ht="17.25">
+      <c r="A138" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B138" s="12"/>
+      <c r="C138" s="12"/>
+      <c r="D138" s="12"/>
+      <c r="E138" s="12"/>
+      <c r="F138" s="12"/>
+      <c r="G138" s="12"/>
+      <c r="H138" s="13"/>
+    </row>
+    <row r="139" spans="1:8" ht="16.5">
+      <c r="A139" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B139" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C139" s="16"/>
+      <c r="D139" s="16"/>
+      <c r="E139" s="16"/>
+      <c r="F139" s="16"/>
+      <c r="G139" s="16"/>
+      <c r="H139" s="17"/>
+    </row>
+    <row r="140" spans="1:8" ht="16.5">
+      <c r="A140" s="1"/>
+      <c r="B140" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C140" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D140" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="E140" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F140" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="G140" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="H140" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="18">
+      <c r="A141" s="2"/>
+      <c r="B141" s="18">
+        <v>46031</v>
+      </c>
+      <c r="C141" s="18">
+        <f>B141+1</f>
+        <v>46032</v>
+      </c>
+      <c r="D141" s="18">
+        <f t="shared" ref="D141:H141" si="0">C141+1</f>
+        <v>46033</v>
+      </c>
+      <c r="E141" s="18">
+        <f t="shared" si="0"/>
+        <v>46034</v>
+      </c>
+      <c r="F141" s="18">
+        <f t="shared" si="0"/>
+        <v>46035</v>
+      </c>
+      <c r="G141" s="18">
+        <f t="shared" si="0"/>
+        <v>46036</v>
+      </c>
+      <c r="H141" s="18">
+        <f t="shared" si="0"/>
+        <v>46037</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="33">
+      <c r="A142" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B142" s="6"/>
+      <c r="C142" s="6"/>
+      <c r="D142" s="6"/>
+      <c r="E142" s="6"/>
+      <c r="F142" s="6"/>
+      <c r="G142" s="6"/>
+      <c r="H142" s="6"/>
+    </row>
+    <row r="143" spans="1:8" ht="16.5">
+      <c r="A143" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B143" s="6"/>
+      <c r="C143" s="6"/>
+      <c r="D143" s="6"/>
+      <c r="E143" s="6"/>
+      <c r="F143" s="6"/>
+      <c r="G143" s="6"/>
+      <c r="H143" s="1"/>
+    </row>
+    <row r="144" spans="1:8" ht="16.5">
+      <c r="A144" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B144" s="6"/>
+      <c r="C144" s="6"/>
+      <c r="D144" s="6"/>
+      <c r="E144" s="7"/>
+      <c r="F144" s="6"/>
+      <c r="G144" s="6"/>
+      <c r="H144" s="1"/>
+    </row>
+    <row r="145" spans="1:8" ht="16.5">
+      <c r="A145" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B145" s="6"/>
+      <c r="C145" s="6"/>
+      <c r="D145" s="6"/>
+      <c r="E145" s="7"/>
+      <c r="F145" s="6"/>
+      <c r="G145" s="6"/>
+      <c r="H145" s="1"/>
+    </row>
+    <row r="146" spans="1:8" ht="49.5">
+      <c r="A146" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B146" s="6"/>
+      <c r="C146" s="1"/>
+      <c r="D146" s="7"/>
+      <c r="E146" s="1"/>
+      <c r="F146" s="1"/>
+      <c r="G146" s="1"/>
+      <c r="H146" s="1"/>
+    </row>
+    <row r="147" spans="1:8" ht="16.5">
+      <c r="A147" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B147" s="1"/>
+      <c r="C147" s="1"/>
+      <c r="D147" s="1"/>
+      <c r="E147" s="1"/>
+      <c r="F147" s="1"/>
+      <c r="G147" s="1"/>
+      <c r="H147" s="1"/>
+    </row>
+    <row r="148" spans="1:8" ht="33">
+      <c r="A148" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B148" s="1"/>
+      <c r="C148" s="1"/>
+      <c r="D148" s="1"/>
+      <c r="E148" s="1"/>
+      <c r="F148" s="1"/>
+      <c r="G148" s="1"/>
+      <c r="H148" s="1"/>
+    </row>
+    <row r="149" spans="1:8" ht="33">
+      <c r="A149" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B149" s="1"/>
+      <c r="C149" s="1"/>
+      <c r="D149" s="1"/>
+      <c r="E149" s="1"/>
+      <c r="F149" s="1"/>
+      <c r="G149" s="1"/>
+      <c r="H149" s="1"/>
+    </row>
+    <row r="150" spans="1:8" ht="82.5">
+      <c r="A150" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B150" s="1"/>
+      <c r="C150" s="1"/>
+      <c r="D150" s="1"/>
+      <c r="E150" s="1"/>
+      <c r="F150" s="1"/>
+      <c r="G150" s="1"/>
+      <c r="H150" s="1"/>
+    </row>
+    <row r="151" spans="1:8" ht="66">
+      <c r="A151" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B151" s="1"/>
+      <c r="C151" s="1"/>
+      <c r="D151" s="1"/>
+      <c r="E151" s="1"/>
+      <c r="F151" s="1"/>
+      <c r="G151" s="1"/>
+      <c r="H151" s="1"/>
+    </row>
+    <row r="152" spans="1:8" ht="49.5">
+      <c r="A152" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B152" s="1"/>
+      <c r="C152" s="1"/>
+      <c r="D152" s="1"/>
+      <c r="E152" s="1"/>
+      <c r="F152" s="1"/>
+      <c r="G152" s="1"/>
+      <c r="H152" s="1"/>
+    </row>
+    <row r="153" spans="1:8" ht="99">
+      <c r="A153" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B153" s="1"/>
+      <c r="C153" s="1"/>
+      <c r="D153" s="1"/>
+      <c r="E153" s="1"/>
+      <c r="F153" s="1"/>
+      <c r="G153" s="1"/>
+      <c r="H153" s="1"/>
+    </row>
+    <row r="154" spans="1:8" ht="115.5">
+      <c r="A154" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B154" s="1"/>
+      <c r="C154" s="1"/>
+      <c r="D154" s="1"/>
+      <c r="E154" s="1"/>
+      <c r="F154" s="1"/>
+      <c r="G154" s="1"/>
+      <c r="H154" s="1"/>
+    </row>
+    <row r="155" spans="1:8" ht="66">
+      <c r="A155" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B155" s="1"/>
+      <c r="C155" s="1"/>
+      <c r="D155" s="1"/>
+      <c r="E155" s="1"/>
+      <c r="F155" s="1"/>
+      <c r="G155" s="1"/>
+      <c r="H155" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="20">
+    <mergeCell ref="A138:H138"/>
+    <mergeCell ref="B139:H139"/>
+    <mergeCell ref="A101:H101"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="A119:H119"/>
+    <mergeCell ref="B120:H120"/>
+    <mergeCell ref="A59:H59"/>
+    <mergeCell ref="B102:H102"/>
+    <mergeCell ref="A79:H79"/>
+    <mergeCell ref="B80:H80"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A60:H60"/>
     <mergeCell ref="A40:H40"/>
@@ -3947,14 +4283,6 @@
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="A41:H41"/>
     <mergeCell ref="B42:H42"/>
-    <mergeCell ref="A101:H101"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="A119:H119"/>
-    <mergeCell ref="B120:H120"/>
-    <mergeCell ref="A59:H59"/>
-    <mergeCell ref="B102:H102"/>
-    <mergeCell ref="A79:H79"/>
-    <mergeCell ref="B80:H80"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
vault backup: 2026-01-10 13:12:52
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary.xlsx
+++ b/睡眠日记_Sleep_Diary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_like\My_like\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8E0001-9F8B-48C5-B61A-77F6A6E80FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83BC3C2-1D9F-47D3-9B75-7CF6D6FF51E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11865" yWindow="225" windowWidth="15705" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="睡眠日记 Sleep Diary" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="156">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -554,6 +554,12 @@
   </si>
   <si>
     <t>第七天</t>
+  </si>
+  <si>
+    <t>未在床上/卧室使用电子设备计算入吗？</t>
+  </si>
+  <si>
+    <t>有 50 min</t>
   </si>
 </sst>
 </file>
@@ -726,14 +732,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -743,8 +749,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1048,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H155"/>
+  <dimension ref="A1:H156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="E145" sqref="E145"/>
+    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B155" sqref="B155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
@@ -1060,28 +1066,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8" ht="16.5">
       <c r="A3" s="1" t="s">
@@ -1489,28 +1495,28 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="13"/>
+      <c r="A21" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" ht="16.5">
       <c r="A23" s="1" t="s">
@@ -1915,28 +1921,28 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="13"/>
+      <c r="A40" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="14"/>
     </row>
     <row r="42" spans="1:8" ht="16.5">
       <c r="A42" s="1" t="s">
@@ -2341,28 +2347,28 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="22.5">
-      <c r="A59" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B59" s="12"/>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
-      <c r="H59" s="13"/>
+      <c r="A59" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="14"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="14" t="s">
+      <c r="A60" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B60" s="12"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="13"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="14"/>
     </row>
     <row r="61" spans="1:8" ht="16.5">
       <c r="A61" s="1" t="s">
@@ -2767,16 +2773,16 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="17.25">
-      <c r="A79" s="14" t="s">
+      <c r="A79" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B79" s="12"/>
-      <c r="C79" s="12"/>
-      <c r="D79" s="12"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
-      <c r="G79" s="12"/>
-      <c r="H79" s="13"/>
+      <c r="B79" s="13"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="14"/>
     </row>
     <row r="80" spans="1:8" ht="16.5">
       <c r="A80" s="1" t="s">
@@ -3186,16 +3192,16 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="17.25">
-      <c r="A101" s="14" t="s">
+      <c r="A101" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B101" s="12"/>
-      <c r="C101" s="12"/>
-      <c r="D101" s="12"/>
-      <c r="E101" s="12"/>
-      <c r="F101" s="12"/>
-      <c r="G101" s="12"/>
-      <c r="H101" s="13"/>
+      <c r="B101" s="13"/>
+      <c r="C101" s="13"/>
+      <c r="D101" s="13"/>
+      <c r="E101" s="13"/>
+      <c r="F101" s="13"/>
+      <c r="G101" s="13"/>
+      <c r="H101" s="14"/>
     </row>
     <row r="102" spans="1:8" ht="16.5">
       <c r="A102" s="1" t="s">
@@ -3600,16 +3606,16 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="17.25">
-      <c r="A119" s="14" t="s">
+      <c r="A119" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B119" s="12"/>
-      <c r="C119" s="12"/>
-      <c r="D119" s="12"/>
-      <c r="E119" s="12"/>
-      <c r="F119" s="12"/>
-      <c r="G119" s="12"/>
-      <c r="H119" s="13"/>
+      <c r="B119" s="13"/>
+      <c r="C119" s="13"/>
+      <c r="D119" s="13"/>
+      <c r="E119" s="13"/>
+      <c r="F119" s="13"/>
+      <c r="G119" s="13"/>
+      <c r="H119" s="14"/>
     </row>
     <row r="120" spans="1:8" ht="16.5">
       <c r="A120" s="1" t="s">
@@ -4014,16 +4020,16 @@
       </c>
     </row>
     <row r="138" spans="1:8" ht="17.25">
-      <c r="A138" s="14" t="s">
+      <c r="A138" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B138" s="12"/>
-      <c r="C138" s="12"/>
-      <c r="D138" s="12"/>
-      <c r="E138" s="12"/>
-      <c r="F138" s="12"/>
-      <c r="G138" s="12"/>
-      <c r="H138" s="13"/>
+      <c r="B138" s="13"/>
+      <c r="C138" s="13"/>
+      <c r="D138" s="13"/>
+      <c r="E138" s="13"/>
+      <c r="F138" s="13"/>
+      <c r="G138" s="13"/>
+      <c r="H138" s="14"/>
     </row>
     <row r="139" spans="1:8" ht="16.5">
       <c r="A139" s="1" t="s">
@@ -4065,39 +4071,41 @@
     </row>
     <row r="141" spans="1:8" ht="18">
       <c r="A141" s="2"/>
-      <c r="B141" s="18">
-        <v>46031</v>
-      </c>
-      <c r="C141" s="18">
+      <c r="B141" s="11">
+        <v>46032</v>
+      </c>
+      <c r="C141" s="11">
         <f>B141+1</f>
-        <v>46032</v>
-      </c>
-      <c r="D141" s="18">
+        <v>46033</v>
+      </c>
+      <c r="D141" s="11">
         <f t="shared" ref="D141:H141" si="0">C141+1</f>
-        <v>46033</v>
-      </c>
-      <c r="E141" s="18">
-        <f t="shared" si="0"/>
         <v>46034</v>
       </c>
-      <c r="F141" s="18">
+      <c r="E141" s="11">
         <f t="shared" si="0"/>
         <v>46035</v>
       </c>
-      <c r="G141" s="18">
+      <c r="F141" s="11">
         <f t="shared" si="0"/>
         <v>46036</v>
       </c>
-      <c r="H141" s="18">
+      <c r="G141" s="11">
         <f t="shared" si="0"/>
         <v>46037</v>
       </c>
+      <c r="H141" s="11">
+        <f t="shared" si="0"/>
+        <v>46038</v>
+      </c>
     </row>
     <row r="142" spans="1:8" ht="33">
       <c r="A142" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B142" s="6"/>
+      <c r="B142" t="s">
+        <v>94</v>
+      </c>
       <c r="C142" s="6"/>
       <c r="D142" s="6"/>
       <c r="E142" s="6"/>
@@ -4109,7 +4117,9 @@
       <c r="A143" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B143" s="6"/>
+      <c r="B143" s="6" t="s">
+        <v>94</v>
+      </c>
       <c r="C143" s="6"/>
       <c r="D143" s="6"/>
       <c r="E143" s="6"/>
@@ -4121,7 +4131,9 @@
       <c r="A144" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B144" s="6"/>
+      <c r="B144" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="C144" s="6"/>
       <c r="D144" s="6"/>
       <c r="E144" s="7"/>
@@ -4133,7 +4145,9 @@
       <c r="A145" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B145" s="6"/>
+      <c r="B145" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="C145" s="6"/>
       <c r="D145" s="6"/>
       <c r="E145" s="7"/>
@@ -4145,7 +4159,9 @@
       <c r="A146" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B146" s="6"/>
+      <c r="B146" s="6">
+        <v>0</v>
+      </c>
       <c r="C146" s="1"/>
       <c r="D146" s="7"/>
       <c r="E146" s="1"/>
@@ -4157,7 +4173,9 @@
       <c r="A147" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B147" s="1"/>
+      <c r="B147" s="1">
+        <v>2</v>
+      </c>
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
@@ -4169,7 +4187,9 @@
       <c r="A148" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B148" s="1"/>
+      <c r="B148" s="1">
+        <v>30</v>
+      </c>
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
@@ -4181,7 +4201,9 @@
       <c r="A149" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B149" s="1"/>
+      <c r="B149" s="1">
+        <v>480</v>
+      </c>
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
@@ -4193,7 +4215,9 @@
       <c r="A150" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B150" s="1"/>
+      <c r="B150" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
       <c r="E150" s="1"/>
@@ -4205,7 +4229,9 @@
       <c r="A151" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B151" s="1"/>
+      <c r="B151" s="1">
+        <v>0</v>
+      </c>
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
       <c r="E151" s="1"/>
@@ -4217,7 +4243,9 @@
       <c r="A152" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B152" s="1"/>
+      <c r="B152" s="1">
+        <v>3</v>
+      </c>
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
       <c r="E152" s="1"/>
@@ -4229,7 +4257,9 @@
       <c r="A153" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B153" s="1"/>
+      <c r="B153" s="1">
+        <v>4</v>
+      </c>
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
       <c r="E153" s="1"/>
@@ -4241,7 +4271,9 @@
       <c r="A154" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B154" s="1"/>
+      <c r="B154" s="1">
+        <v>4</v>
+      </c>
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
       <c r="E154" s="1"/>
@@ -4253,7 +4285,9 @@
       <c r="A155" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B155" s="1"/>
+      <c r="B155" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
       <c r="E155" s="1"/>
@@ -4261,14 +4295,13 @@
       <c r="G155" s="1"/>
       <c r="H155" s="1"/>
     </row>
+    <row r="156" spans="1:8">
+      <c r="B156" t="s">
+        <v>154</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A138:H138"/>
-    <mergeCell ref="B139:H139"/>
-    <mergeCell ref="A101:H101"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="A119:H119"/>
-    <mergeCell ref="B120:H120"/>
     <mergeCell ref="A59:H59"/>
     <mergeCell ref="B102:H102"/>
     <mergeCell ref="A79:H79"/>
@@ -4283,7 +4316,22 @@
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="A41:H41"/>
     <mergeCell ref="B42:H42"/>
+    <mergeCell ref="A138:H138"/>
+    <mergeCell ref="B139:H139"/>
+    <mergeCell ref="A101:H101"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="A119:H119"/>
+    <mergeCell ref="B120:H120"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter>
+    <oddFooter>&amp;L_x000D_&amp;1#&amp;"Aptos"&amp;10&amp;K000000 Classified as Internal | Intern</oddFooter>
+  </headerFooter>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{d465f887-04a9-4c17-8b62-103eddccf68b}" enabled="1" method="Standard" siteId="{ca2a7f76-dbd7-4ec0-9108-6b3d524fb7c8}" contentBits="2" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
vault backup: 2026-01-12 15:14:47
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary.xlsx
+++ b/睡眠日记_Sleep_Diary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_like\My_like\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83BC3C2-1D9F-47D3-9B75-7CF6D6FF51E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3321937-CB43-4677-84E2-9BA88828C2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11865" yWindow="225" windowWidth="15705" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="睡眠日记 Sleep Diary" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="159">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -560,6 +560,15 @@
   </si>
   <si>
     <t>有 50 min</t>
+  </si>
+  <si>
+    <t>8：51</t>
+  </si>
+  <si>
+    <t>21：30</t>
+  </si>
+  <si>
+    <t>有 60 min</t>
   </si>
 </sst>
 </file>
@@ -735,7 +744,7 @@
     <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -749,7 +758,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1056,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B155" sqref="B155"/>
+    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
@@ -1066,7 +1075,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="13"/>
@@ -1078,7 +1087,7 @@
       <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="13"/>
@@ -1495,7 +1504,7 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="13"/>
@@ -1507,7 +1516,7 @@
       <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="13"/>
@@ -1921,7 +1930,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="18" t="s">
+      <c r="A40" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="13"/>
@@ -1933,7 +1942,7 @@
       <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="13"/>
@@ -2347,7 +2356,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="22.5">
-      <c r="A59" s="18" t="s">
+      <c r="A59" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="13"/>
@@ -2359,7 +2368,7 @@
       <c r="H59" s="14"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="12" t="s">
+      <c r="A60" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="13"/>
@@ -2773,7 +2782,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="17.25">
-      <c r="A79" s="12" t="s">
+      <c r="A79" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B79" s="13"/>
@@ -3192,7 +3201,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="17.25">
-      <c r="A101" s="12" t="s">
+      <c r="A101" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B101" s="13"/>
@@ -3606,7 +3615,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="17.25">
-      <c r="A119" s="12" t="s">
+      <c r="A119" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B119" s="13"/>
@@ -4020,7 +4029,7 @@
       </c>
     </row>
     <row r="138" spans="1:8" ht="17.25">
-      <c r="A138" s="12" t="s">
+      <c r="A138" s="18" t="s">
         <v>1</v>
       </c>
       <c r="B138" s="13"/>
@@ -4106,8 +4115,12 @@
       <c r="B142" t="s">
         <v>94</v>
       </c>
-      <c r="C142" s="6"/>
-      <c r="D142" s="6"/>
+      <c r="C142" s="6">
+        <v>0.3125</v>
+      </c>
+      <c r="D142" s="6" t="s">
+        <v>156</v>
+      </c>
       <c r="E142" s="6"/>
       <c r="F142" s="6"/>
       <c r="G142" s="6"/>
@@ -4120,8 +4133,12 @@
       <c r="B143" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C143" s="6"/>
-      <c r="D143" s="6"/>
+      <c r="C143" s="6">
+        <v>0.31944444444444442</v>
+      </c>
+      <c r="D143" s="6" t="s">
+        <v>72</v>
+      </c>
       <c r="E143" s="6"/>
       <c r="F143" s="6"/>
       <c r="G143" s="6"/>
@@ -4134,8 +4151,12 @@
       <c r="B144" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C144" s="6"/>
-      <c r="D144" s="6"/>
+      <c r="C144" s="6">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D144" s="6" t="s">
+        <v>157</v>
+      </c>
       <c r="E144" s="7"/>
       <c r="F144" s="6"/>
       <c r="G144" s="6"/>
@@ -4148,8 +4169,12 @@
       <c r="B145" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C145" s="6"/>
-      <c r="D145" s="6"/>
+      <c r="C145" s="6">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D145" s="6" t="s">
+        <v>157</v>
+      </c>
       <c r="E145" s="7"/>
       <c r="F145" s="6"/>
       <c r="G145" s="6"/>
@@ -4162,8 +4187,12 @@
       <c r="B146" s="6">
         <v>0</v>
       </c>
-      <c r="C146" s="1"/>
-      <c r="D146" s="7"/>
+      <c r="C146" s="1">
+        <v>0</v>
+      </c>
+      <c r="D146" s="7">
+        <v>0</v>
+      </c>
       <c r="E146" s="1"/>
       <c r="F146" s="1"/>
       <c r="G146" s="1"/>
@@ -4176,8 +4205,12 @@
       <c r="B147" s="1">
         <v>2</v>
       </c>
-      <c r="C147" s="1"/>
-      <c r="D147" s="1"/>
+      <c r="C147" s="1">
+        <v>1</v>
+      </c>
+      <c r="D147" s="1">
+        <v>3</v>
+      </c>
       <c r="E147" s="1"/>
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
@@ -4190,8 +4223,12 @@
       <c r="B148" s="1">
         <v>30</v>
       </c>
-      <c r="C148" s="1"/>
-      <c r="D148" s="1"/>
+      <c r="C148" s="1">
+        <v>5</v>
+      </c>
+      <c r="D148" s="1">
+        <v>30</v>
+      </c>
       <c r="E148" s="1"/>
       <c r="F148" s="1"/>
       <c r="G148" s="1"/>
@@ -4204,8 +4241,12 @@
       <c r="B149" s="1">
         <v>480</v>
       </c>
-      <c r="C149" s="1"/>
-      <c r="D149" s="1"/>
+      <c r="C149" s="1">
+        <v>510</v>
+      </c>
+      <c r="D149" s="1">
+        <v>600</v>
+      </c>
       <c r="E149" s="1"/>
       <c r="F149" s="1"/>
       <c r="G149" s="1"/>
@@ -4218,8 +4259,12 @@
       <c r="B150" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C150" s="1"/>
-      <c r="D150" s="1"/>
+      <c r="C150" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D150" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="E150" s="1"/>
       <c r="F150" s="1"/>
       <c r="G150" s="1"/>
@@ -4232,8 +4277,12 @@
       <c r="B151" s="1">
         <v>0</v>
       </c>
-      <c r="C151" s="1"/>
-      <c r="D151" s="1"/>
+      <c r="C151" s="1">
+        <v>0</v>
+      </c>
+      <c r="D151" s="1">
+        <v>0</v>
+      </c>
       <c r="E151" s="1"/>
       <c r="F151" s="1"/>
       <c r="G151" s="1"/>
@@ -4246,8 +4295,12 @@
       <c r="B152" s="1">
         <v>3</v>
       </c>
-      <c r="C152" s="1"/>
-      <c r="D152" s="1"/>
+      <c r="C152" s="1">
+        <v>4</v>
+      </c>
+      <c r="D152" s="1">
+        <v>3</v>
+      </c>
       <c r="E152" s="1"/>
       <c r="F152" s="1"/>
       <c r="G152" s="1"/>
@@ -4260,8 +4313,12 @@
       <c r="B153" s="1">
         <v>4</v>
       </c>
-      <c r="C153" s="1"/>
-      <c r="D153" s="1"/>
+      <c r="C153" s="1">
+        <v>4</v>
+      </c>
+      <c r="D153" s="1">
+        <v>4</v>
+      </c>
       <c r="E153" s="1"/>
       <c r="F153" s="1"/>
       <c r="G153" s="1"/>
@@ -4274,8 +4331,12 @@
       <c r="B154" s="1">
         <v>4</v>
       </c>
-      <c r="C154" s="1"/>
-      <c r="D154" s="1"/>
+      <c r="C154" s="1">
+        <v>4</v>
+      </c>
+      <c r="D154" s="1">
+        <v>3</v>
+      </c>
       <c r="E154" s="1"/>
       <c r="F154" s="1"/>
       <c r="G154" s="1"/>
@@ -4288,9 +4349,15 @@
       <c r="B155" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C155" s="1"/>
-      <c r="D155" s="1"/>
-      <c r="E155" s="1"/>
+      <c r="C155" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E155" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="F155" s="1"/>
       <c r="G155" s="1"/>
       <c r="H155" s="1"/>
@@ -4302,6 +4369,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A138:H138"/>
+    <mergeCell ref="B139:H139"/>
+    <mergeCell ref="A101:H101"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="A119:H119"/>
+    <mergeCell ref="B120:H120"/>
     <mergeCell ref="A59:H59"/>
     <mergeCell ref="B102:H102"/>
     <mergeCell ref="A79:H79"/>
@@ -4316,12 +4389,6 @@
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="A41:H41"/>
     <mergeCell ref="B42:H42"/>
-    <mergeCell ref="A138:H138"/>
-    <mergeCell ref="B139:H139"/>
-    <mergeCell ref="A101:H101"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="A119:H119"/>
-    <mergeCell ref="B120:H120"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>

</xml_diff>

<commit_message>
vault backup: 2026-01-13 10:45:47
</commit_message>
<xml_diff>
--- a/睡眠日记_Sleep_Diary.xlsx
+++ b/睡眠日记_Sleep_Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\My_lovwly\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3321937-CB43-4677-84E2-9BA88828C2EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADD7B2C-89A3-4E02-A84C-9E0AA7AF8CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11865" yWindow="225" windowWidth="15705" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="160">
   <si>
     <t>睡眠日记 Sleep Diary</t>
   </si>
@@ -569,6 +569,9 @@
   </si>
   <si>
     <t>有 60 min</t>
+  </si>
+  <si>
+    <t>7：51</t>
   </si>
 </sst>
 </file>
@@ -744,7 +747,7 @@
     <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -758,7 +761,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1065,8 +1068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="C157" sqref="C157"/>
+    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="F153" sqref="F153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="15"/>
@@ -1075,7 +1078,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22.5">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="13"/>
@@ -1087,7 +1090,7 @@
       <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" ht="17.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="13"/>
@@ -1504,7 +1507,7 @@
       <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:8" ht="22.5">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="13"/>
@@ -1516,7 +1519,7 @@
       <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8" ht="17.25">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="13"/>
@@ -1930,7 +1933,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="22.5">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="13"/>
@@ -1942,7 +1945,7 @@
       <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" ht="17.25">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="13"/>
@@ -2356,7 +2359,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="22.5">
-      <c r="A59" s="12" t="s">
+      <c r="A59" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B59" s="13"/>
@@ -2368,7 +2371,7 @@
       <c r="H59" s="14"/>
     </row>
     <row r="60" spans="1:8" ht="17.25">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="13"/>
@@ -2782,7 +2785,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="17.25">
-      <c r="A79" s="18" t="s">
+      <c r="A79" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B79" s="13"/>
@@ -3201,7 +3204,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" ht="17.25">
-      <c r="A101" s="18" t="s">
+      <c r="A101" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B101" s="13"/>
@@ -3615,7 +3618,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="17.25">
-      <c r="A119" s="18" t="s">
+      <c r="A119" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B119" s="13"/>
@@ -4029,7 +4032,7 @@
       </c>
     </row>
     <row r="138" spans="1:8" ht="17.25">
-      <c r="A138" s="18" t="s">
+      <c r="A138" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B138" s="13"/>
@@ -4121,7 +4124,9 @@
       <c r="D142" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="E142" s="6"/>
+      <c r="E142" s="6" t="s">
+        <v>159</v>
+      </c>
       <c r="F142" s="6"/>
       <c r="G142" s="6"/>
       <c r="H142" s="6"/>
@@ -4139,7 +4144,9 @@
       <c r="D143" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E143" s="6"/>
+      <c r="E143" s="6" t="s">
+        <v>15</v>
+      </c>
       <c r="F143" s="6"/>
       <c r="G143" s="6"/>
       <c r="H143" s="1"/>
@@ -4157,7 +4164,9 @@
       <c r="D144" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="E144" s="7"/>
+      <c r="E144" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="F144" s="6"/>
       <c r="G144" s="6"/>
       <c r="H144" s="1"/>
@@ -4175,7 +4184,9 @@
       <c r="D145" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="E145" s="7"/>
+      <c r="E145" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="F145" s="6"/>
       <c r="G145" s="6"/>
       <c r="H145" s="1"/>
@@ -4193,7 +4204,9 @@
       <c r="D146" s="7">
         <v>0</v>
       </c>
-      <c r="E146" s="1"/>
+      <c r="E146" s="1">
+        <v>5</v>
+      </c>
       <c r="F146" s="1"/>
       <c r="G146" s="1"/>
       <c r="H146" s="1"/>
@@ -4211,7 +4224,9 @@
       <c r="D147" s="1">
         <v>3</v>
       </c>
-      <c r="E147" s="1"/>
+      <c r="E147" s="1">
+        <v>1</v>
+      </c>
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
@@ -4229,7 +4244,9 @@
       <c r="D148" s="1">
         <v>30</v>
       </c>
-      <c r="E148" s="1"/>
+      <c r="E148" s="1">
+        <v>5</v>
+      </c>
       <c r="F148" s="1"/>
       <c r="G148" s="1"/>
       <c r="H148" s="1"/>
@@ -4247,7 +4264,9 @@
       <c r="D149" s="1">
         <v>600</v>
       </c>
-      <c r="E149" s="1"/>
+      <c r="E149" s="1">
+        <v>520</v>
+      </c>
       <c r="F149" s="1"/>
       <c r="G149" s="1"/>
       <c r="H149" s="1"/>
@@ -4265,7 +4284,9 @@
       <c r="D150" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E150" s="1"/>
+      <c r="E150" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F150" s="1"/>
       <c r="G150" s="1"/>
       <c r="H150" s="1"/>
@@ -4283,7 +4304,9 @@
       <c r="D151" s="1">
         <v>0</v>
       </c>
-      <c r="E151" s="1"/>
+      <c r="E151" s="1">
+        <v>0</v>
+      </c>
       <c r="F151" s="1"/>
       <c r="G151" s="1"/>
       <c r="H151" s="1"/>
@@ -4301,7 +4324,9 @@
       <c r="D152" s="1">
         <v>3</v>
       </c>
-      <c r="E152" s="1"/>
+      <c r="E152" s="1">
+        <v>4</v>
+      </c>
       <c r="F152" s="1"/>
       <c r="G152" s="1"/>
       <c r="H152" s="1"/>
@@ -4319,7 +4344,9 @@
       <c r="D153" s="1">
         <v>4</v>
       </c>
-      <c r="E153" s="1"/>
+      <c r="E153" s="1">
+        <v>3</v>
+      </c>
       <c r="F153" s="1"/>
       <c r="G153" s="1"/>
       <c r="H153" s="1"/>
@@ -4337,7 +4364,9 @@
       <c r="D154" s="1">
         <v>3</v>
       </c>
-      <c r="E154" s="1"/>
+      <c r="E154" s="1">
+        <v>4</v>
+      </c>
       <c r="F154" s="1"/>
       <c r="G154" s="1"/>
       <c r="H154" s="1"/>
@@ -4369,12 +4398,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A138:H138"/>
-    <mergeCell ref="B139:H139"/>
-    <mergeCell ref="A101:H101"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="A119:H119"/>
-    <mergeCell ref="B120:H120"/>
     <mergeCell ref="A59:H59"/>
     <mergeCell ref="B102:H102"/>
     <mergeCell ref="A79:H79"/>
@@ -4389,6 +4412,12 @@
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="A41:H41"/>
     <mergeCell ref="B42:H42"/>
+    <mergeCell ref="A138:H138"/>
+    <mergeCell ref="B139:H139"/>
+    <mergeCell ref="A101:H101"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="A119:H119"/>
+    <mergeCell ref="B120:H120"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>

</xml_diff>